<commit_message>
raspa outro indicador CAGR dos indicadores de crescimento
</commit_message>
<xml_diff>
--- a/raspagem/empresas_com_indicadores.xlsx
+++ b/raspagem/empresas_com_indicadores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,7 +446,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>crescimento</t>
+          <t>CAGR RECEITAS 5 ANOS</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>CAGR LUCROS 5 ANOS</t>
         </is>
       </c>
     </row>
@@ -469,6 +474,11 @@
           <t>16,29%</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>34,44%</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -489,6 +499,11 @@
           <t>9,68%</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>46,18%</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -509,6 +524,11 @@
           <t>13,44%</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2,56%</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -529,6 +549,11 @@
           <t>13,37%</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>3,10%</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -549,6 +574,11 @@
           <t>66,77%</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>-%</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -569,6 +599,11 @@
           <t>-7,54%</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>-26,63%</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -589,6 +624,11 @@
           <t>16,21%</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>-18,77%</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -609,6 +649,11 @@
           <t>19,06%</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>40,17%</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -629,6 +674,11 @@
           <t>16,61%</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>12,88%</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -649,6 +699,11 @@
           <t>25,49%</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>20,02%</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -669,6 +724,11 @@
           <t>29,83%</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>47,94%</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -689,6 +749,11 @@
           <t>10,72%</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>15,72%</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -709,6 +774,11 @@
           <t>17,75%</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>-%</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -729,6 +799,11 @@
           <t>14,97%</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>24,47%</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -749,6 +824,11 @@
           <t>16,96%</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>14,10%</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -769,6 +849,11 @@
           <t>14,61%</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>-%</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -789,6 +874,11 @@
           <t>36,49%</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>56,62%</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -809,6 +899,11 @@
           <t>17,72%</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>-%</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -829,6 +924,11 @@
           <t>36,49%</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>56,62%</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -847,6 +947,11 @@
       <c r="D21" t="inlineStr">
         <is>
           <t>30,59%</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>54,84%</t>
         </is>
       </c>
     </row>

</xml_diff>